<commit_message>
Cucumber lessons are added.
</commit_message>
<xml_diff>
--- a/target/test-classes/ulkeler.xlsx
+++ b/target/test-classes/ulkeler.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="578">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1753,6 +1753,9 @@
   </si>
   <si>
     <t>54000</t>
+  </si>
+  <si>
+    <t>ulke nufusu</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2221,8 +2224,8 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>574</v>
+      <c r="E2" t="n" s="0">
+        <v>1.5E9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -2307,6 +2310,9 @@
       </c>
       <c r="D8" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>2.5E8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>